<commit_message>
update some data columns
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Heinz\DABP\DABP-Project-Decarbonization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\DABP\Project\DABP-Project-Decarbonization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAB5EDF-C82D-4F98-BAE5-94D06FEBC2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9171D5-34E9-42BA-8ACD-4054DC47CF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7956" yWindow="7716" windowWidth="17280" windowHeight="8964" xr2:uid="{F0F53EF8-A26C-449E-B23E-1CDBC92CF5F3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{F0F53EF8-A26C-449E-B23E-1CDBC92CF5F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>coal</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,29 +66,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>capacity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>generation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>capacity %</t>
-  </si>
-  <si>
-    <t>generation %</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>number</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>fixed_cost(dollar_kW)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>revenues(dollor_kWh)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -95,6 +79,38 @@
   </si>
   <si>
     <t>co2(pounds_kWh)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>source</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>capacity_%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>generation_%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>capacity_national_twh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>generation_national_twh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>capacity_plant_twh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed_cost_power_dollar_kW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed_cost_plant_dollar_kW</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -102,7 +118,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,27 +181,30 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,290 +520,357 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2105060-DB75-474D-9A30-25ACFDAB3F82}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.4140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.9140625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="22.58203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.58203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.25" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.58203125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:12" ht="28">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
+      <c r="C2" s="1">
+        <f>I2/B2</f>
+        <v>7.5345854999999995</v>
+      </c>
+      <c r="D2" s="1">
+        <v>750</v>
+      </c>
+      <c r="E2" s="1">
+        <f>C2*D2*10^9</f>
+        <v>5650939125000</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="I2" s="1">
+        <f>87.1/1000*365*24*K2</f>
+        <v>60.276683999999996</v>
+      </c>
+      <c r="J2" s="1">
+        <f t="shared" ref="J2:J8" si="0">222.6*L2</f>
+        <v>13.8012</v>
+      </c>
+      <c r="K2" s="5">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="L2" s="5">
+        <v>6.2E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:12">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C8" si="1">I3/B3</f>
+        <v>2.14592625</v>
+      </c>
+      <c r="D3" s="1">
+        <v>600</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E8" si="2">C3*D3*10^9</f>
+        <v>1287555750000</v>
+      </c>
+      <c r="F3" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I8" si="3">87.1/1000*365*24*K3</f>
+        <v>103.00446000000001</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" si="0"/>
+        <v>22.705199999999998</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="1"/>
+        <v>5.7390568695652169</v>
+      </c>
+      <c r="D4" s="1">
+        <v>900</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="2"/>
+        <v>5165151182608.6953</v>
+      </c>
+      <c r="F4" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="3"/>
+        <v>131.99830799999998</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="0"/>
+        <v>51.6432</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.23200000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="1"/>
+        <v>7.248462</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3100</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="2"/>
+        <v>22470232200000</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="H5" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>750</v>
-      </c>
-      <c r="D2">
-        <v>0.03</v>
-      </c>
-      <c r="E2">
+      <c r="I5" s="1">
+        <f t="shared" si="3"/>
+        <v>28.993848</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="0"/>
+        <v>25.599</v>
+      </c>
+      <c r="K5" s="5">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>739</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.33039069012178618</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3100</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="2"/>
+        <v>1024211139377.5371</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G6" s="1">
         <v>0.32</v>
       </c>
-      <c r="F2">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="G2">
-        <f>87.1/1000*365*24*I2</f>
-        <v>60.276683999999996</v>
-      </c>
-      <c r="H2">
-        <f>222.6*J2</f>
-        <v>13.8012</v>
-      </c>
-      <c r="I2" s="4">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="J2" s="4">
-        <v>6.2E-2</v>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="3"/>
+        <v>244.15871999999999</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>56.985599999999998</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0.32</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0.25600000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>48</v>
-      </c>
-      <c r="C3">
-        <v>600</v>
-      </c>
-      <c r="D3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E3">
+    <row r="7" spans="1:12">
+      <c r="A7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>256</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.50965748437500002</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3100</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="2"/>
+        <v>1579938201562.5002</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G7" s="1">
         <v>0.32</v>
       </c>
-      <c r="F3">
-        <v>0.97</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G8" si="0">87.1/1000*365*24*I3</f>
-        <v>103.00446000000001</v>
-      </c>
-      <c r="H3">
-        <f>222.6*J3</f>
-        <v>22.705199999999998</v>
-      </c>
-      <c r="I3" s="4">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0.10199999999999999</v>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="3"/>
+        <v>130.47231600000001</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
+        <v>37.841999999999999</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0.17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>23</v>
-      </c>
-      <c r="C4">
-        <v>900</v>
-      </c>
-      <c r="D4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E4">
+    <row r="8" spans="1:12">
+      <c r="A8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>141</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.39502629787234039</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4500</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="2"/>
+        <v>1777618340425.532</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G8" s="1">
         <v>0.32</v>
       </c>
-      <c r="F4">
-        <v>0.77</v>
-      </c>
-      <c r="G4">
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="3"/>
+        <v>55.698707999999996</v>
+      </c>
+      <c r="J8" s="1">
         <f t="shared" si="0"/>
-        <v>131.99830799999998</v>
-      </c>
-      <c r="H4">
-        <f>222.6*J4</f>
-        <v>51.6432</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0.17299999999999999</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0.23200000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>3100</v>
-      </c>
-      <c r="D5">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="E5">
-        <v>0.32</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>28.993848</v>
-      </c>
-      <c r="H5">
-        <f>222.6*J5</f>
-        <v>25.599</v>
-      </c>
-      <c r="I5" s="4">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0.115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>739</v>
-      </c>
-      <c r="C6">
-        <v>3100</v>
-      </c>
-      <c r="D6">
-        <v>0.01</v>
-      </c>
-      <c r="E6">
-        <v>0.32</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>244.15871999999999</v>
-      </c>
-      <c r="H6">
-        <f>222.6*J6</f>
-        <v>56.985599999999998</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0.32</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0.25600000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>256</v>
-      </c>
-      <c r="C7">
-        <v>3100</v>
-      </c>
-      <c r="D7">
-        <v>0.01</v>
-      </c>
-      <c r="E7">
-        <v>0.32</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>130.47231600000001</v>
-      </c>
-      <c r="H7">
-        <f>222.6*J7</f>
-        <v>37.841999999999999</v>
-      </c>
-      <c r="I7" s="4">
-        <v>0.17100000000000001</v>
-      </c>
-      <c r="J7" s="4">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>141</v>
-      </c>
-      <c r="C8">
-        <v>4500</v>
-      </c>
-      <c r="D8">
-        <v>0.01</v>
-      </c>
-      <c r="E8">
-        <v>0.32</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>55.698707999999996</v>
-      </c>
-      <c r="H8">
-        <f>222.6*J8</f>
         <v>7.7910000000000004</v>
       </c>
-      <c r="I8" s="4">
+      <c r="K8" s="5">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="J8" s="4">
+      <c r="L8" s="5">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
split change of plants dv into add and minus
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Heinz\DABP\DABP-Project-Decarbonization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\DABP\Project\DABP-Project-Decarbonization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D020B6D2-32A3-4093-8CF8-81CC9BBFA73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A37A413-5042-4EE9-8E4F-9E95223E18F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{F0F53EF8-A26C-449E-B23E-1CDBC92CF5F3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{F0F53EF8-A26C-449E-B23E-1CDBC92CF5F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -107,11 +110,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>capacity_plant_kwh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>fixed_cost_plant_dollar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>capacity_plant_kw</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -119,7 +122,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -524,26 +527,26 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.4140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="22.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.9140625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="22.58203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="24" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.21875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" style="1" customWidth="1"/>
-    <col min="9" max="10" width="29.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.58203125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="29.25" style="1" customWidth="1"/>
     <col min="11" max="11" width="18.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.58203125" style="1" customWidth="1"/>
     <col min="14" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="28">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -551,13 +554,13 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>9</v>
@@ -584,7 +587,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -630,7 +633,7 @@
         <v>6.2E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -658,7 +661,7 @@
         <v>0.97</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:J8" si="3">87.1/1000*365*24*L3</f>
+        <f t="shared" ref="I3:I8" si="3">87.1/1000*365*24*L3</f>
         <v>103.00446000000001</v>
       </c>
       <c r="J3" s="1">
@@ -676,7 +679,7 @@
         <v>0.10199999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -722,7 +725,7 @@
         <v>0.23200000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -768,7 +771,7 @@
         <v>0.115</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -814,7 +817,7 @@
         <v>0.25600000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
@@ -860,7 +863,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="6" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Updated data.csv and data.xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Heinz\DABP\DABP-Project-Decarbonization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2676FB71-9C57-4DB0-90CF-3EF7D5D4FA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4436D838-10C2-41C7-AC06-7D18F274F50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{F0F53EF8-A26C-449E-B23E-1CDBC92CF5F3}"/>
   </bookViews>
@@ -119,6 +119,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -182,7 +185,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -198,13 +201,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -524,7 +524,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -588,45 +588,45 @@
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="6">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="6">
         <f>J2/B2</f>
         <v>860112.5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="6">
         <v>750</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="6">
         <f>C2*D2</f>
         <v>645084375</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="6">
         <v>0.03</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="6">
         <v>0.32</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="6">
         <v>2.2599999999999998</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="6">
         <f>87.1*10^6*365*24*L2</f>
         <v>60276684000</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="6">
         <f>87.1*L2*10^6</f>
         <v>6880900</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="6">
         <f>222.6*M2*10^9</f>
         <v>13801200000</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="6">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="6">
         <v>6.2E-2</v>
       </c>
     </row>
@@ -634,45 +634,45 @@
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="6">
         <v>48</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="6">
         <f t="shared" ref="C3:C8" si="0">J3/B3</f>
         <v>244968.75</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="6">
         <v>600</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="6">
         <f t="shared" ref="E3:E8" si="1">C3*D3</f>
         <v>146981250</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="6">
         <v>0.32</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="6">
         <v>0.97</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="6">
         <f t="shared" ref="I3:I8" si="2">87.1*10^6*365*24*L3</f>
         <v>103004460000</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="6">
         <f t="shared" ref="J3:J8" si="3">87.1*L3*10^6</f>
         <v>11758500</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="6">
         <f t="shared" ref="K3:K8" si="4">222.6*M3*10^9</f>
         <v>22705199999.999996</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="6">
         <v>0.13500000000000001</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="6">
         <v>0.10199999999999999</v>
       </c>
     </row>
@@ -680,229 +680,229 @@
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="6">
         <v>23</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="6">
         <f t="shared" si="0"/>
         <v>655143.47826086939</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="6">
         <v>900</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="6">
         <f t="shared" si="1"/>
         <v>589629130.43478251</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="6">
         <v>0.32</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="6">
         <v>0.77</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="6">
         <f t="shared" si="2"/>
         <v>131998307999.99998</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="6">
         <f t="shared" si="3"/>
         <v>15068299.999999996</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="6">
         <f t="shared" si="4"/>
         <v>51643200000</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="6">
         <v>0.17299999999999999</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="6">
         <v>0.23200000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="6">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="6">
         <f t="shared" si="0"/>
         <v>827449.99999999988</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="6">
         <v>3100</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="6">
         <f t="shared" si="1"/>
         <v>2565094999.9999995</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="6">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="6">
         <v>0.32</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="6">
         <v>0</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="6">
         <f t="shared" si="2"/>
         <v>28993848000</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="6">
         <f t="shared" si="3"/>
         <v>3309799.9999999995</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="6">
         <f t="shared" si="4"/>
         <v>25599000000</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="6">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="6">
         <v>0.115</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="6">
         <v>739</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="6">
         <f t="shared" si="0"/>
         <v>37715.832205683357</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="6">
         <v>3100</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="6">
         <f t="shared" si="1"/>
         <v>116919079.83761841</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="6">
         <v>0.01</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="6">
         <v>0.32</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="6">
         <v>0</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="6">
         <f t="shared" si="2"/>
         <v>244158720000</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="6">
         <f t="shared" si="3"/>
         <v>27872000</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="6">
         <f t="shared" si="4"/>
         <v>56985600000</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="6">
         <v>0.32</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="6">
         <v>0.25600000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="6">
         <v>256</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="6">
         <f t="shared" si="0"/>
         <v>58180.078125</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="6">
         <v>3100</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="6">
         <f t="shared" si="1"/>
         <v>180358242.1875</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="6">
         <v>0.01</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="6">
         <v>0.32</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="6">
         <v>0</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="6">
         <f t="shared" si="2"/>
         <v>130472316000.00002</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="6">
         <f t="shared" si="3"/>
         <v>14894100</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="6">
         <f t="shared" si="4"/>
         <v>37842000000</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="6">
         <v>0.17100000000000001</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="6">
         <v>0.17</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="6">
         <v>141</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="6">
         <f t="shared" si="0"/>
         <v>45094.326241134746</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="6">
         <v>4500</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="6">
         <f t="shared" si="1"/>
         <v>202924468.08510634</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="6">
         <v>0.01</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="6">
         <v>0.32</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="6">
         <v>0</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="6">
         <f t="shared" si="2"/>
         <v>55698708000</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="6">
         <f t="shared" si="3"/>
         <v>6358299.9999999991</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="6">
         <f t="shared" si="4"/>
         <v>7791000000</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="6">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="6">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Solution for the first time!
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Heinz\DABP\DABP-Project-Decarbonization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\DABP\Project\DABP-Project-Decarbonization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4436D838-10C2-41C7-AC06-7D18F274F50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D17AB1-61B2-4E03-AB29-148186F807E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{F0F53EF8-A26C-449E-B23E-1CDBC92CF5F3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{F0F53EF8-A26C-449E-B23E-1CDBC92CF5F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>coal</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -99,10 +102,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>capacity_plant_kw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>capacity_national_kwh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -112,6 +111,22 @@
   </si>
   <si>
     <t>generation_national_kwh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>load_factor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plant_capacity_power_kw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plant_capacity_force_kwh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plant_generate_force_kwh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -122,7 +137,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -521,29 +536,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2105060-DB75-474D-9A30-25ACFDAB3F82}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.4140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="22.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.21875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" style="1" customWidth="1"/>
-    <col min="9" max="10" width="29.21875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.6640625" style="1"/>
+    <col min="3" max="3" width="22.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.9140625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="22.58203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.25" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.58203125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="29.25" style="1" customWidth="1"/>
+    <col min="13" max="14" width="18.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.58203125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="28">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -551,40 +568,49 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -592,45 +618,57 @@
         <v>8</v>
       </c>
       <c r="C2" s="6">
-        <f>J2/B2</f>
+        <f>L2/B2</f>
         <v>860112.5</v>
       </c>
       <c r="D2" s="6">
+        <f>C2* 365 * 24</f>
+        <v>7534585500</v>
+      </c>
+      <c r="E2" s="6">
+        <f>D2*N2</f>
+        <v>1725150000</v>
+      </c>
+      <c r="F2" s="6">
         <v>750</v>
       </c>
-      <c r="E2" s="6">
-        <f>C2*D2</f>
+      <c r="G2" s="6">
+        <f>C2*F2</f>
         <v>645084375</v>
       </c>
-      <c r="F2" s="6">
+      <c r="H2" s="6">
         <v>0.03</v>
       </c>
-      <c r="G2" s="6">
+      <c r="I2" s="6">
         <v>0.32</v>
       </c>
-      <c r="H2" s="6">
+      <c r="J2" s="6">
         <v>2.2599999999999998</v>
       </c>
-      <c r="I2" s="6">
-        <f>87.1*10^6*365*24*L2</f>
+      <c r="K2" s="6">
+        <f>87.1*10^6*365*24*O2</f>
         <v>60276684000</v>
       </c>
-      <c r="J2" s="6">
-        <f>87.1*L2*10^6</f>
+      <c r="L2" s="6">
+        <f>87.1*O2*10^6</f>
         <v>6880900</v>
       </c>
-      <c r="K2" s="6">
-        <f>222.6*M2*10^9</f>
+      <c r="M2" s="6">
+        <f>222.6*P2*10^9</f>
         <v>13801200000</v>
       </c>
-      <c r="L2" s="6">
+      <c r="N2" s="6">
+        <f>M2/K2</f>
+        <v>0.2289641546970301</v>
+      </c>
+      <c r="O2" s="6">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="M2" s="6">
+      <c r="P2" s="6">
         <v>6.2E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -638,45 +676,57 @@
         <v>48</v>
       </c>
       <c r="C3" s="6">
-        <f t="shared" ref="C3:C8" si="0">J3/B3</f>
+        <f t="shared" ref="C3:C8" si="0">L3/B3</f>
         <v>244968.75</v>
       </c>
       <c r="D3" s="6">
+        <f t="shared" ref="D3:D8" si="1">C3* 365 * 24</f>
+        <v>2145926250</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E8" si="2">D3*N3</f>
+        <v>473024999.99999994</v>
+      </c>
+      <c r="F3" s="6">
         <v>600</v>
       </c>
-      <c r="E3" s="6">
-        <f t="shared" ref="E3:E8" si="1">C3*D3</f>
+      <c r="G3" s="6">
+        <f t="shared" ref="G3:G8" si="3">C3*F3</f>
         <v>146981250</v>
       </c>
-      <c r="F3" s="6">
+      <c r="H3" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G3" s="6">
+      <c r="I3" s="6">
         <v>0.32</v>
       </c>
-      <c r="H3" s="6">
+      <c r="J3" s="6">
         <v>0.97</v>
       </c>
-      <c r="I3" s="6">
-        <f t="shared" ref="I3:I8" si="2">87.1*10^6*365*24*L3</f>
+      <c r="K3" s="6">
+        <f t="shared" ref="K3:K8" si="4">87.1*10^6*365*24*O3</f>
         <v>103004460000</v>
       </c>
-      <c r="J3" s="6">
-        <f t="shared" ref="J3:J8" si="3">87.1*L3*10^6</f>
+      <c r="L3" s="6">
+        <f t="shared" ref="L3:L8" si="5">87.1*O3*10^6</f>
         <v>11758500</v>
       </c>
-      <c r="K3" s="6">
-        <f t="shared" ref="K3:K8" si="4">222.6*M3*10^9</f>
+      <c r="M3" s="6">
+        <f t="shared" ref="M3:M8" si="6">222.6*P3*10^9</f>
         <v>22705199999.999996</v>
       </c>
-      <c r="L3" s="6">
+      <c r="N3" s="6">
+        <f t="shared" ref="N3:N8" si="7">M3/K3</f>
+        <v>0.2204292901491838</v>
+      </c>
+      <c r="O3" s="6">
         <v>0.13500000000000001</v>
       </c>
-      <c r="M3" s="6">
+      <c r="P3" s="6">
         <v>0.10199999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -688,41 +738,53 @@
         <v>655143.47826086939</v>
       </c>
       <c r="D4" s="6">
+        <f t="shared" si="1"/>
+        <v>5739056869.5652161</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="2"/>
+        <v>2245356521.73913</v>
+      </c>
+      <c r="F4" s="6">
         <v>900</v>
       </c>
-      <c r="E4" s="6">
-        <f t="shared" si="1"/>
+      <c r="G4" s="6">
+        <f t="shared" si="3"/>
         <v>589629130.43478251</v>
       </c>
-      <c r="F4" s="6">
+      <c r="H4" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G4" s="6">
+      <c r="I4" s="6">
         <v>0.32</v>
       </c>
-      <c r="H4" s="6">
+      <c r="J4" s="6">
         <v>0.77</v>
-      </c>
-      <c r="I4" s="6">
-        <f t="shared" si="2"/>
-        <v>131998307999.99998</v>
-      </c>
-      <c r="J4" s="6">
-        <f t="shared" si="3"/>
-        <v>15068299.999999996</v>
       </c>
       <c r="K4" s="6">
         <f t="shared" si="4"/>
+        <v>131998307999.99998</v>
+      </c>
+      <c r="L4" s="6">
+        <f t="shared" si="5"/>
+        <v>15068299.999999996</v>
+      </c>
+      <c r="M4" s="6">
+        <f t="shared" si="6"/>
         <v>51643200000</v>
       </c>
-      <c r="L4" s="6">
+      <c r="N4" s="6">
+        <f t="shared" si="7"/>
+        <v>0.39124137863948988</v>
+      </c>
+      <c r="O4" s="6">
         <v>0.17299999999999999</v>
       </c>
-      <c r="M4" s="6">
+      <c r="P4" s="6">
         <v>0.23200000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -734,41 +796,53 @@
         <v>827449.99999999988</v>
       </c>
       <c r="D5" s="6">
+        <f t="shared" si="1"/>
+        <v>7248461999.9999981</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="2"/>
+        <v>6399749999.999999</v>
+      </c>
+      <c r="F5" s="6">
         <v>3100</v>
       </c>
-      <c r="E5" s="6">
-        <f t="shared" si="1"/>
+      <c r="G5" s="6">
+        <f t="shared" si="3"/>
         <v>2565094999.9999995</v>
       </c>
-      <c r="F5" s="6">
+      <c r="H5" s="6">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="G5" s="6">
+      <c r="I5" s="6">
         <v>0.32</v>
       </c>
-      <c r="H5" s="6">
+      <c r="J5" s="6">
         <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <f t="shared" si="2"/>
-        <v>28993848000</v>
-      </c>
-      <c r="J5" s="6">
-        <f t="shared" si="3"/>
-        <v>3309799.9999999995</v>
       </c>
       <c r="K5" s="6">
         <f t="shared" si="4"/>
+        <v>28993848000</v>
+      </c>
+      <c r="L5" s="6">
+        <f t="shared" si="5"/>
+        <v>3309799.9999999995</v>
+      </c>
+      <c r="M5" s="6">
+        <f t="shared" si="6"/>
         <v>25599000000</v>
       </c>
-      <c r="L5" s="6">
+      <c r="N5" s="6">
+        <f t="shared" si="7"/>
+        <v>0.88291143693655294</v>
+      </c>
+      <c r="O5" s="6">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="M5" s="6">
+      <c r="P5" s="6">
         <v>0.115</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -780,41 +854,53 @@
         <v>37715.832205683357</v>
       </c>
       <c r="D6" s="6">
+        <f t="shared" si="1"/>
+        <v>330390690.12178618</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="2"/>
+        <v>77111772.66576454</v>
+      </c>
+      <c r="F6" s="6">
         <v>3100</v>
       </c>
-      <c r="E6" s="6">
-        <f t="shared" si="1"/>
+      <c r="G6" s="6">
+        <f t="shared" si="3"/>
         <v>116919079.83761841</v>
       </c>
-      <c r="F6" s="6">
+      <c r="H6" s="6">
         <v>0.01</v>
       </c>
-      <c r="G6" s="6">
+      <c r="I6" s="6">
         <v>0.32</v>
       </c>
-      <c r="H6" s="6">
+      <c r="J6" s="6">
         <v>0</v>
-      </c>
-      <c r="I6" s="6">
-        <f t="shared" si="2"/>
-        <v>244158720000</v>
-      </c>
-      <c r="J6" s="6">
-        <f t="shared" si="3"/>
-        <v>27872000</v>
       </c>
       <c r="K6" s="6">
         <f t="shared" si="4"/>
+        <v>244158720000</v>
+      </c>
+      <c r="L6" s="6">
+        <f t="shared" si="5"/>
+        <v>27872000</v>
+      </c>
+      <c r="M6" s="6">
+        <f t="shared" si="6"/>
         <v>56985600000</v>
       </c>
-      <c r="L6" s="6">
+      <c r="N6" s="6">
+        <f t="shared" si="7"/>
+        <v>0.23339571898148875</v>
+      </c>
+      <c r="O6" s="6">
         <v>0.32</v>
       </c>
-      <c r="M6" s="6">
+      <c r="P6" s="6">
         <v>0.25600000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
@@ -826,41 +912,53 @@
         <v>58180.078125</v>
       </c>
       <c r="D7" s="6">
+        <f t="shared" si="1"/>
+        <v>509657484.375</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="2"/>
+        <v>147820312.49999997</v>
+      </c>
+      <c r="F7" s="6">
         <v>3100</v>
       </c>
-      <c r="E7" s="6">
-        <f t="shared" si="1"/>
+      <c r="G7" s="6">
+        <f t="shared" si="3"/>
         <v>180358242.1875</v>
       </c>
-      <c r="F7" s="6">
+      <c r="H7" s="6">
         <v>0.01</v>
       </c>
-      <c r="G7" s="6">
+      <c r="I7" s="6">
         <v>0.32</v>
       </c>
-      <c r="H7" s="6">
+      <c r="J7" s="6">
         <v>0</v>
-      </c>
-      <c r="I7" s="6">
-        <f t="shared" si="2"/>
-        <v>130472316000.00002</v>
-      </c>
-      <c r="J7" s="6">
-        <f t="shared" si="3"/>
-        <v>14894100</v>
       </c>
       <c r="K7" s="6">
         <f t="shared" si="4"/>
+        <v>130472316000.00002</v>
+      </c>
+      <c r="L7" s="6">
+        <f t="shared" si="5"/>
+        <v>14894100</v>
+      </c>
+      <c r="M7" s="6">
+        <f t="shared" si="6"/>
         <v>37842000000</v>
       </c>
-      <c r="L7" s="6">
+      <c r="N7" s="6">
+        <f t="shared" si="7"/>
+        <v>0.29003853966997867</v>
+      </c>
+      <c r="O7" s="6">
         <v>0.17100000000000001</v>
       </c>
-      <c r="M7" s="6">
+      <c r="P7" s="6">
         <v>0.17</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
@@ -872,37 +970,49 @@
         <v>45094.326241134746</v>
       </c>
       <c r="D8" s="6">
+        <f t="shared" si="1"/>
+        <v>395026297.87234038</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="2"/>
+        <v>55255319.14893616</v>
+      </c>
+      <c r="F8" s="6">
         <v>4500</v>
       </c>
-      <c r="E8" s="6">
-        <f t="shared" si="1"/>
+      <c r="G8" s="6">
+        <f t="shared" si="3"/>
         <v>202924468.08510634</v>
       </c>
-      <c r="F8" s="6">
+      <c r="H8" s="6">
         <v>0.01</v>
       </c>
-      <c r="G8" s="6">
+      <c r="I8" s="6">
         <v>0.32</v>
       </c>
-      <c r="H8" s="6">
+      <c r="J8" s="6">
         <v>0</v>
-      </c>
-      <c r="I8" s="6">
-        <f t="shared" si="2"/>
-        <v>55698708000</v>
-      </c>
-      <c r="J8" s="6">
-        <f t="shared" si="3"/>
-        <v>6358299.9999999991</v>
       </c>
       <c r="K8" s="6">
         <f t="shared" si="4"/>
+        <v>55698708000</v>
+      </c>
+      <c r="L8" s="6">
+        <f t="shared" si="5"/>
+        <v>6358299.9999999991</v>
+      </c>
+      <c r="M8" s="6">
+        <f t="shared" si="6"/>
         <v>7791000000</v>
       </c>
-      <c r="L8" s="6">
+      <c r="N8" s="6">
+        <f t="shared" si="7"/>
+        <v>0.13987757130739908</v>
+      </c>
+      <c r="O8" s="6">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="M8" s="6">
+      <c r="P8" s="6">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>

</xml_diff>